<commit_message>
sent gordon data showing alltoallv is bad at scaling. Need to get isend/irecv going
</commit_message>
<xml_diff>
--- a/latex/performance_content/scaling/strong_scaling.xlsx
+++ b/latex/performance_content/scaling/strong_scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20140" yWindow="0" windowWidth="30100" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50420" windowHeight="28360" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Unoptimized Nested Loop" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,11 @@
     <sheet name="ViennaCL" sheetId="3" r:id="rId4"/>
     <sheet name="clSpMV" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId6"/>
+    <sheet name="IMPI_vs_OMPI" sheetId="7" r:id="rId7"/>
+    <sheet name="IMPI_4M" sheetId="8" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Strong scaling</t>
   </si>
@@ -127,6 +129,12 @@
   <si>
     <t>Efficiency</t>
   </si>
+  <si>
+    <t>IMPI</t>
+  </si>
+  <si>
+    <t>4096000 Nodes</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +194,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,6 +299,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -302,7 +354,7 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="104">
+  <cellStyles count="148">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +406,28 @@
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +479,28 @@
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="21" builtinId="5"/>
   </cellStyles>
@@ -558,7 +654,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -658,7 +754,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
@@ -758,7 +854,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
@@ -858,7 +954,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
@@ -1062,6 +1158,456 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time (ms) per SpMV</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (N=160^3 points, with IMPI; MPI_Alltoallv Collective)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_4M!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=17</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_4M!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>65.5447</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.7078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.3822</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.5659</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.04806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.38003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.22125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.07608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.483814</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.182466</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_4M!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_4M!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>103.241</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_4M!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_4M!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_4M!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=101</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_4M!$E$4:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2136267064"/>
+        <c:axId val="-2136159528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2136267064"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Count (8 ppn)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2136159528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2136159528"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2136267064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -1102,12 +1648,22 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.059415790001916"/>
+          <c:y val="0.086183574879227"/>
+          <c:w val="0.831730184943568"/>
+          <c:h val="0.818460648940621"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -1207,7 +1763,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -1307,7 +1863,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
@@ -1407,7 +1963,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
@@ -3793,6 +4349,1111 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time (ms) per SpMV</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (N=100^3 points, with IMPI; MPI_Alltoallv Collective)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Unoptimized Nested Loop'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=17</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$C$7:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>31.8092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.8514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.9811</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.51561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.23287</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.27062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.37328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5856</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.68299</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.41328</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Unoptimized Nested Loop'!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$E$7:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>53.0019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.0028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.0799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.6617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.4283</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.62684</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.07126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.89876</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.45455</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.06669</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.66918</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Unoptimized Nested Loop'!$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$G$7:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>73.8507</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.7232</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.5457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.7056</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.2133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.91594</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.52578</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.67407</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.44322</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.48035</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.90961</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Unoptimized Nested Loop'!$I$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=101</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$A$7:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Unoptimized Nested Loop'!$I$7:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>168.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.0309</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.1105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.3044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.8746</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.6801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.03172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.19303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.01938</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.06002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.33263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2145915816"/>
+        <c:axId val="2145000648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2145915816"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Count (8 ppn)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145000648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2145000648"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2145915816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time (ms) per SpMV</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (N=100^3 points, with OMPI; MPI_Alltoallv Collective)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1797111340225"/>
+          <c:y val="0.0154589371980676"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_vs_OMPI!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=17</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>38.4957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.5125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.9081</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.2782</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.37736</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.13064</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.32408</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.28543</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.45031</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.67413</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.41363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_vs_OMPI!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>51.7426</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.9618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.2704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.6102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.15178</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.38237</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.30406</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.56914</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.40594</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.26382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_vs_OMPI!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>91.9445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.9798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.106</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.6211</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.9932</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.812</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.40634</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.49497</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5615</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.07249</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.8134</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IMPI_vs_OMPI!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n=101</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IMPI_vs_OMPI!$E$4:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>151.106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.07899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.9425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50.9381</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.6588</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.367</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.3694</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.33143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.25437</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7351</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2140641208"/>
+        <c:axId val="2146042600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2140641208"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Count (8 ppn)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146042600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2146042600"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2140641208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -4030,6 +5691,112 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4601,8 +6368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5802,4 +7569,372 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>38.495699999999999</v>
+      </c>
+      <c r="C4">
+        <v>51.742600000000003</v>
+      </c>
+      <c r="D4">
+        <v>91.944500000000005</v>
+      </c>
+      <c r="E4">
+        <v>151.10599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>26.512499999999999</v>
+      </c>
+      <c r="C5">
+        <v>31.9618</v>
+      </c>
+      <c r="D5">
+        <v>56.979799999999997</v>
+      </c>
+      <c r="E5">
+        <v>99.078999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>18.908100000000001</v>
+      </c>
+      <c r="C6">
+        <v>30.270399999999999</v>
+      </c>
+      <c r="D6">
+        <v>39.106000000000002</v>
+      </c>
+      <c r="E6">
+        <v>88.942499999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>14.2782</v>
+      </c>
+      <c r="C7">
+        <v>18.468</v>
+      </c>
+      <c r="D7">
+        <v>29.621099999999998</v>
+      </c>
+      <c r="E7">
+        <v>50.938099999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>9.3773599999999995</v>
+      </c>
+      <c r="C8">
+        <v>14.610200000000001</v>
+      </c>
+      <c r="D8">
+        <v>17.993200000000002</v>
+      </c>
+      <c r="E8">
+        <v>32.658799999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>5.1306399999999996</v>
+      </c>
+      <c r="C9">
+        <v>7.1517799999999996</v>
+      </c>
+      <c r="D9">
+        <v>11.811999999999999</v>
+      </c>
+      <c r="E9">
+        <v>18.367000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>3.3240799999999999</v>
+      </c>
+      <c r="C10">
+        <v>4.3823699999999999</v>
+      </c>
+      <c r="D10">
+        <v>6.4063400000000001</v>
+      </c>
+      <c r="E10">
+        <v>11.369400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>2.2854299999999999</v>
+      </c>
+      <c r="C11">
+        <v>3.3040600000000002</v>
+      </c>
+      <c r="D11">
+        <v>4.4949700000000004</v>
+      </c>
+      <c r="E11">
+        <v>6.3314300000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>1.45031</v>
+      </c>
+      <c r="C12">
+        <v>2.56914</v>
+      </c>
+      <c r="D12">
+        <v>2.5615000000000001</v>
+      </c>
+      <c r="E12">
+        <v>4.2543699999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>512</v>
+      </c>
+      <c r="B13">
+        <v>1.6741299999999999</v>
+      </c>
+      <c r="C13">
+        <v>1.40594</v>
+      </c>
+      <c r="D13">
+        <v>2.0724900000000002</v>
+      </c>
+      <c r="E13">
+        <v>3.7351000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <v>2.4136299999999999</v>
+      </c>
+      <c r="C14">
+        <v>3.2638199999999999</v>
+      </c>
+      <c r="D14">
+        <v>2.8134000000000001</v>
+      </c>
+      <c r="E14">
+        <v>3.7593999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>65.544700000000006</v>
+      </c>
+      <c r="C5">
+        <v>103.241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>47.707799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>36.382199999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>17.565899999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>9.0480599999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>4.3800299999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>2.2212499999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>1.0760799999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>512</v>
+      </c>
+      <c r="B13">
+        <v>0.48381400000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <v>0.18246599999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>